<commit_message>
[Document, Modified]: TaskList(2) Specification and Login-Logout Specification
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/Login-Logout/Login_Logout Specification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/Login-Logout/Login_Logout Specification.xlsx
@@ -387,10 +387,10 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -443,13 +443,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -472,134 +476,136 @@
   <dimension ref="B3:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="14.46"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -633,143 +639,145 @@
   <dimension ref="B3:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="14.46"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="58.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="70.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
+    <row r="11" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="78.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -803,179 +811,181 @@
   <dimension ref="B3:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="14.46"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="78.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="83.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="93.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1009,143 +1019,145 @@
   <dimension ref="B3:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="14.46"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="76.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1179,143 +1191,145 @@
   <dimension ref="B3:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="14.46"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="99.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="103.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="47" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1349,143 +1363,145 @@
   <dimension ref="B3:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="14.46"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="95.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="102" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="97" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1519,152 +1535,154 @@
   <dimension ref="B3:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="58.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="14.46"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="1" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>